<commit_message>
Just added my personal data files
</commit_message>
<xml_diff>
--- a/data/felix/output/processed_f.xlsx
+++ b/data/felix/output/processed_f.xlsx
@@ -527,54 +527,52 @@
         </is>
       </c>
       <c r="B2" t="n">
-        <v>-76.66</v>
+        <v>-80.38</v>
       </c>
       <c r="C2" t="n">
-        <v>0</v>
+        <v>528.72</v>
       </c>
       <c r="D2" t="n">
-        <v>0</v>
+        <v>50</v>
       </c>
       <c r="E2" t="n">
-        <v>0</v>
+        <v>0.41</v>
       </c>
       <c r="F2" t="n">
-        <v>-84.34999999999999</v>
+        <v>-82.81999999999999</v>
       </c>
       <c r="G2" t="n">
-        <v>0</v>
+        <v>528.72</v>
       </c>
       <c r="H2" t="n">
-        <v>0</v>
+        <v>50</v>
       </c>
       <c r="I2" t="n">
-        <v>0</v>
+        <v>0.4</v>
       </c>
       <c r="J2" t="n">
-        <v>-25.64</v>
+        <v>-26.88</v>
       </c>
       <c r="K2" t="n">
-        <v>0</v>
+        <v>528.72</v>
       </c>
       <c r="L2" t="n">
-        <v>0</v>
+        <v>50</v>
       </c>
       <c r="M2" t="n">
-        <v>0</v>
+        <v>1.24</v>
       </c>
       <c r="N2" t="n">
-        <v>216620.11</v>
+        <v>43392.34</v>
       </c>
       <c r="O2" t="n">
-        <v>83.34</v>
-      </c>
-      <c r="P2" t="inlineStr">
-        <is>
-          <t>inf</t>
-        </is>
+        <v>113.4</v>
+      </c>
+      <c r="P2" t="n">
+        <v>51.23</v>
       </c>
       <c r="Q2" t="n">
-        <v>9</v>
+        <v>6.61</v>
       </c>
     </row>
     <row r="3">
@@ -584,54 +582,52 @@
         </is>
       </c>
       <c r="B3" t="n">
-        <v>-85.36</v>
+        <v>-90.65000000000001</v>
       </c>
       <c r="C3" t="n">
-        <v>0</v>
+        <v>528.72</v>
       </c>
       <c r="D3" t="n">
-        <v>0</v>
+        <v>50</v>
       </c>
       <c r="E3" t="n">
-        <v>0</v>
+        <v>0.37</v>
       </c>
       <c r="F3" t="n">
-        <v>-82.69</v>
+        <v>-89.84</v>
       </c>
       <c r="G3" t="n">
-        <v>0</v>
+        <v>528.72</v>
       </c>
       <c r="H3" t="n">
-        <v>0</v>
+        <v>50</v>
       </c>
       <c r="I3" t="n">
-        <v>0</v>
+        <v>0.37</v>
       </c>
       <c r="J3" t="n">
-        <v>-28.55</v>
+        <v>-30.32</v>
       </c>
       <c r="K3" t="n">
-        <v>0</v>
+        <v>528.72</v>
       </c>
       <c r="L3" t="n">
-        <v>0</v>
+        <v>50</v>
       </c>
       <c r="M3" t="n">
-        <v>0</v>
+        <v>1.1</v>
       </c>
       <c r="N3" t="n">
-        <v>216620.11</v>
+        <v>43392.34</v>
       </c>
       <c r="O3" t="n">
-        <v>83.34</v>
-      </c>
-      <c r="P3" t="inlineStr">
-        <is>
-          <t>inf</t>
-        </is>
+        <v>113.4</v>
+      </c>
+      <c r="P3" t="n">
+        <v>51.23</v>
       </c>
       <c r="Q3" t="n">
-        <v>9</v>
+        <v>6.61</v>
       </c>
     </row>
     <row r="4">
@@ -641,54 +637,52 @@
         </is>
       </c>
       <c r="B4" t="n">
-        <v>-85.01000000000001</v>
+        <v>-90.37</v>
       </c>
       <c r="C4" t="n">
-        <v>0</v>
+        <v>528.72</v>
       </c>
       <c r="D4" t="n">
-        <v>0</v>
+        <v>50</v>
       </c>
       <c r="E4" t="n">
-        <v>0</v>
+        <v>0.37</v>
       </c>
       <c r="F4" t="n">
-        <v>-82.06999999999999</v>
+        <v>-90.11</v>
       </c>
       <c r="G4" t="n">
-        <v>0</v>
+        <v>528.72</v>
       </c>
       <c r="H4" t="n">
-        <v>0</v>
+        <v>50</v>
       </c>
       <c r="I4" t="n">
-        <v>0</v>
+        <v>0.37</v>
       </c>
       <c r="J4" t="n">
-        <v>-28.43</v>
+        <v>-30.23</v>
       </c>
       <c r="K4" t="n">
-        <v>0</v>
+        <v>528.72</v>
       </c>
       <c r="L4" t="n">
-        <v>0</v>
+        <v>50</v>
       </c>
       <c r="M4" t="n">
-        <v>0</v>
+        <v>1.1</v>
       </c>
       <c r="N4" t="n">
-        <v>216620.11</v>
+        <v>43392.34</v>
       </c>
       <c r="O4" t="n">
-        <v>83.34</v>
-      </c>
-      <c r="P4" t="inlineStr">
-        <is>
-          <t>inf</t>
-        </is>
+        <v>113.4</v>
+      </c>
+      <c r="P4" t="n">
+        <v>51.23</v>
       </c>
       <c r="Q4" t="n">
-        <v>9</v>
+        <v>6.61</v>
       </c>
     </row>
     <row r="5">
@@ -698,54 +692,52 @@
         </is>
       </c>
       <c r="B5" t="n">
-        <v>-84.56999999999999</v>
+        <v>-89.84</v>
       </c>
       <c r="C5" t="n">
-        <v>0</v>
+        <v>528.72</v>
       </c>
       <c r="D5" t="n">
-        <v>0</v>
+        <v>50</v>
       </c>
       <c r="E5" t="n">
-        <v>0</v>
+        <v>0.37</v>
       </c>
       <c r="F5" t="n">
-        <v>-82.01000000000001</v>
+        <v>-89.86</v>
       </c>
       <c r="G5" t="n">
-        <v>0</v>
+        <v>528.72</v>
       </c>
       <c r="H5" t="n">
-        <v>0</v>
+        <v>50</v>
       </c>
       <c r="I5" t="n">
-        <v>0</v>
+        <v>0.37</v>
       </c>
       <c r="J5" t="n">
-        <v>-28.29</v>
+        <v>-30.05</v>
       </c>
       <c r="K5" t="n">
-        <v>0</v>
+        <v>528.72</v>
       </c>
       <c r="L5" t="n">
-        <v>0</v>
+        <v>50</v>
       </c>
       <c r="M5" t="n">
-        <v>0</v>
+        <v>1.11</v>
       </c>
       <c r="N5" t="n">
-        <v>216620.11</v>
+        <v>43392.34</v>
       </c>
       <c r="O5" t="n">
-        <v>83.34</v>
-      </c>
-      <c r="P5" t="inlineStr">
-        <is>
-          <t>inf</t>
-        </is>
+        <v>113.4</v>
+      </c>
+      <c r="P5" t="n">
+        <v>51.23</v>
       </c>
       <c r="Q5" t="n">
-        <v>9</v>
+        <v>6.61</v>
       </c>
     </row>
     <row r="6">
@@ -755,54 +747,52 @@
         </is>
       </c>
       <c r="B6" t="n">
-        <v>-84.41</v>
+        <v>-89.62</v>
       </c>
       <c r="C6" t="n">
-        <v>0</v>
+        <v>528.72</v>
       </c>
       <c r="D6" t="n">
-        <v>0</v>
+        <v>50</v>
       </c>
       <c r="E6" t="n">
-        <v>0</v>
+        <v>0.37</v>
       </c>
       <c r="F6" t="n">
-        <v>-81.93000000000001</v>
+        <v>-89.68000000000001</v>
       </c>
       <c r="G6" t="n">
-        <v>0</v>
+        <v>528.72</v>
       </c>
       <c r="H6" t="n">
-        <v>0</v>
+        <v>50</v>
       </c>
       <c r="I6" t="n">
-        <v>0</v>
+        <v>0.37</v>
       </c>
       <c r="J6" t="n">
-        <v>-28.23</v>
+        <v>-29.97</v>
       </c>
       <c r="K6" t="n">
-        <v>0</v>
+        <v>528.72</v>
       </c>
       <c r="L6" t="n">
-        <v>0</v>
+        <v>50</v>
       </c>
       <c r="M6" t="n">
-        <v>0</v>
+        <v>1.11</v>
       </c>
       <c r="N6" t="n">
-        <v>216620.11</v>
+        <v>43392.34</v>
       </c>
       <c r="O6" t="n">
-        <v>83.34</v>
-      </c>
-      <c r="P6" t="inlineStr">
-        <is>
-          <t>inf</t>
-        </is>
+        <v>113.4</v>
+      </c>
+      <c r="P6" t="n">
+        <v>51.23</v>
       </c>
       <c r="Q6" t="n">
-        <v>9</v>
+        <v>6.61</v>
       </c>
     </row>
     <row r="7">
@@ -812,54 +802,52 @@
         </is>
       </c>
       <c r="B7" t="n">
-        <v>-84.56999999999999</v>
+        <v>-89.84</v>
       </c>
       <c r="C7" t="n">
-        <v>0</v>
+        <v>528.72</v>
       </c>
       <c r="D7" t="n">
-        <v>0</v>
+        <v>50</v>
       </c>
       <c r="E7" t="n">
-        <v>0</v>
+        <v>0.37</v>
       </c>
       <c r="F7" t="n">
-        <v>-82.01000000000001</v>
+        <v>-89.86</v>
       </c>
       <c r="G7" t="n">
-        <v>0</v>
+        <v>528.72</v>
       </c>
       <c r="H7" t="n">
-        <v>0</v>
+        <v>50</v>
       </c>
       <c r="I7" t="n">
-        <v>0</v>
+        <v>0.37</v>
       </c>
       <c r="J7" t="n">
-        <v>-28.29</v>
+        <v>-30.05</v>
       </c>
       <c r="K7" t="n">
-        <v>0</v>
+        <v>528.72</v>
       </c>
       <c r="L7" t="n">
-        <v>0</v>
+        <v>50</v>
       </c>
       <c r="M7" t="n">
-        <v>0</v>
+        <v>1.11</v>
       </c>
       <c r="N7" t="n">
-        <v>216620.11</v>
+        <v>43392.34</v>
       </c>
       <c r="O7" t="n">
-        <v>83.34</v>
-      </c>
-      <c r="P7" t="inlineStr">
-        <is>
-          <t>inf</t>
-        </is>
+        <v>113.4</v>
+      </c>
+      <c r="P7" t="n">
+        <v>51.23</v>
       </c>
       <c r="Q7" t="n">
-        <v>9</v>
+        <v>6.61</v>
       </c>
     </row>
     <row r="8">
@@ -869,54 +857,52 @@
         </is>
       </c>
       <c r="B8" t="n">
-        <v>-85.01000000000001</v>
+        <v>-90.37</v>
       </c>
       <c r="C8" t="n">
-        <v>0</v>
+        <v>528.72</v>
       </c>
       <c r="D8" t="n">
-        <v>0</v>
+        <v>50</v>
       </c>
       <c r="E8" t="n">
-        <v>0</v>
+        <v>0.37</v>
       </c>
       <c r="F8" t="n">
-        <v>-82.06999999999999</v>
+        <v>-90.11</v>
       </c>
       <c r="G8" t="n">
-        <v>0</v>
+        <v>528.72</v>
       </c>
       <c r="H8" t="n">
-        <v>0</v>
+        <v>50</v>
       </c>
       <c r="I8" t="n">
-        <v>0</v>
+        <v>0.37</v>
       </c>
       <c r="J8" t="n">
-        <v>-28.43</v>
+        <v>-30.23</v>
       </c>
       <c r="K8" t="n">
-        <v>0</v>
+        <v>528.72</v>
       </c>
       <c r="L8" t="n">
-        <v>0</v>
+        <v>50</v>
       </c>
       <c r="M8" t="n">
-        <v>0</v>
+        <v>1.1</v>
       </c>
       <c r="N8" t="n">
-        <v>216620.11</v>
+        <v>43392.34</v>
       </c>
       <c r="O8" t="n">
-        <v>83.34</v>
-      </c>
-      <c r="P8" t="inlineStr">
-        <is>
-          <t>inf</t>
-        </is>
+        <v>113.4</v>
+      </c>
+      <c r="P8" t="n">
+        <v>51.23</v>
       </c>
       <c r="Q8" t="n">
-        <v>9</v>
+        <v>6.61</v>
       </c>
     </row>
     <row r="9">
@@ -926,54 +912,52 @@
         </is>
       </c>
       <c r="B9" t="n">
-        <v>-85.36</v>
+        <v>-90.65000000000001</v>
       </c>
       <c r="C9" t="n">
-        <v>0</v>
+        <v>528.72</v>
       </c>
       <c r="D9" t="n">
-        <v>0</v>
+        <v>50</v>
       </c>
       <c r="E9" t="n">
-        <v>0</v>
+        <v>0.37</v>
       </c>
       <c r="F9" t="n">
-        <v>-82.69</v>
+        <v>-89.84</v>
       </c>
       <c r="G9" t="n">
-        <v>0</v>
+        <v>528.72</v>
       </c>
       <c r="H9" t="n">
-        <v>0</v>
+        <v>50</v>
       </c>
       <c r="I9" t="n">
-        <v>0</v>
+        <v>0.37</v>
       </c>
       <c r="J9" t="n">
-        <v>-28.55</v>
+        <v>-30.32</v>
       </c>
       <c r="K9" t="n">
-        <v>0</v>
+        <v>528.72</v>
       </c>
       <c r="L9" t="n">
-        <v>0</v>
+        <v>50</v>
       </c>
       <c r="M9" t="n">
-        <v>0</v>
+        <v>1.1</v>
       </c>
       <c r="N9" t="n">
-        <v>216620.11</v>
+        <v>43392.34</v>
       </c>
       <c r="O9" t="n">
-        <v>83.34</v>
-      </c>
-      <c r="P9" t="inlineStr">
-        <is>
-          <t>inf</t>
-        </is>
+        <v>113.4</v>
+      </c>
+      <c r="P9" t="n">
+        <v>51.23</v>
       </c>
       <c r="Q9" t="n">
-        <v>9</v>
+        <v>6.61</v>
       </c>
     </row>
     <row r="10">
@@ -983,54 +967,52 @@
         </is>
       </c>
       <c r="B10" t="n">
-        <v>-76.66</v>
+        <v>-80.38</v>
       </c>
       <c r="C10" t="n">
-        <v>0</v>
+        <v>528.72</v>
       </c>
       <c r="D10" t="n">
-        <v>0</v>
+        <v>50</v>
       </c>
       <c r="E10" t="n">
-        <v>0</v>
+        <v>0.41</v>
       </c>
       <c r="F10" t="n">
-        <v>-84.34999999999999</v>
+        <v>-82.81999999999999</v>
       </c>
       <c r="G10" t="n">
-        <v>0</v>
+        <v>528.72</v>
       </c>
       <c r="H10" t="n">
-        <v>0</v>
+        <v>50</v>
       </c>
       <c r="I10" t="n">
-        <v>0</v>
+        <v>0.4</v>
       </c>
       <c r="J10" t="n">
-        <v>-25.64</v>
+        <v>-26.88</v>
       </c>
       <c r="K10" t="n">
-        <v>0</v>
+        <v>528.72</v>
       </c>
       <c r="L10" t="n">
-        <v>0</v>
+        <v>50</v>
       </c>
       <c r="M10" t="n">
-        <v>0</v>
+        <v>1.24</v>
       </c>
       <c r="N10" t="n">
-        <v>216620.11</v>
+        <v>43392.34</v>
       </c>
       <c r="O10" t="n">
-        <v>83.34</v>
-      </c>
-      <c r="P10" t="inlineStr">
-        <is>
-          <t>inf</t>
-        </is>
+        <v>113.4</v>
+      </c>
+      <c r="P10" t="n">
+        <v>51.23</v>
       </c>
       <c r="Q10" t="n">
-        <v>9</v>
+        <v>6.61</v>
       </c>
     </row>
   </sheetData>

</xml_diff>